<commit_message>
last commit for spring
</commit_message>
<xml_diff>
--- a/Project Final/Product Backlog-20-Smart_Shop.xlsx
+++ b/Project Final/Product Backlog-20-Smart_Shop.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" checkCompatibility="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\289610\Desktop\Product Backlogs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\smartShop\Project Final\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -123,7 +123,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="280">
   <si>
     <t>Date</t>
   </si>
@@ -1566,6 +1566,9 @@
   </si>
   <si>
     <t>FS 26 / Req_20.1 to 20.5</t>
+  </si>
+  <si>
+    <t>Complete</t>
   </si>
 </sst>
 </file>
@@ -2149,7 +2152,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="190">
+  <cellXfs count="191">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -2460,6 +2463,27 @@
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2517,6 +2541,21 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -2538,21 +2577,6 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2611,26 +2635,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="29" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -2639,8 +2645,36 @@
     <cellStyle name="Normal 2 2" xfId="2"/>
     <cellStyle name="Normal 2 3" xfId="3"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -2723,13 +2757,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>3.9000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>3.6000000000000005</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>3.6000000000000005</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2895,10 +2929,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.3</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -3142,7 +3176,9 @@
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="1"/>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+              </c:ext>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -3212,6 +3248,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -3260,10 +3297,11 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Chart8"/>
   <sheetViews>
-    <sheetView zoomScale="91" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="118" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </chartsheet>
 </file>
 
@@ -3271,10 +3309,11 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Chart9"/>
   <sheetViews>
-    <sheetView zoomScale="71" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="118" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </chartsheet>
 </file>
 
@@ -4746,7 +4785,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8656236" cy="6280220"/>
+    <xdr:ext cx="8669364" cy="6288114"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -5043,7 +5082,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8679824" cy="6291866"/>
+    <xdr:ext cx="8669364" cy="6288114"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -5677,72 +5716,72 @@
       <c r="G5" s="51"/>
     </row>
     <row r="6" spans="2:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="136"/>
-      <c r="C6" s="137"/>
-      <c r="D6" s="137"/>
-      <c r="E6" s="137"/>
-      <c r="F6" s="137"/>
-      <c r="G6" s="138"/>
+      <c r="B6" s="143"/>
+      <c r="C6" s="144"/>
+      <c r="D6" s="144"/>
+      <c r="E6" s="144"/>
+      <c r="F6" s="144"/>
+      <c r="G6" s="145"/>
     </row>
     <row r="7" spans="2:7" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="136"/>
-      <c r="C7" s="137"/>
-      <c r="D7" s="137"/>
-      <c r="E7" s="137"/>
-      <c r="F7" s="137"/>
-      <c r="G7" s="138"/>
+      <c r="B7" s="143"/>
+      <c r="C7" s="144"/>
+      <c r="D7" s="144"/>
+      <c r="E7" s="144"/>
+      <c r="F7" s="144"/>
+      <c r="G7" s="145"/>
     </row>
     <row r="8" spans="2:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="136" t="s">
+      <c r="B8" s="143" t="s">
         <v>164</v>
       </c>
-      <c r="C8" s="137"/>
-      <c r="D8" s="137"/>
-      <c r="E8" s="137"/>
-      <c r="F8" s="137"/>
-      <c r="G8" s="138"/>
+      <c r="C8" s="144"/>
+      <c r="D8" s="144"/>
+      <c r="E8" s="144"/>
+      <c r="F8" s="144"/>
+      <c r="G8" s="145"/>
     </row>
     <row r="9" spans="2:7" ht="23.25" x14ac:dyDescent="0.2">
-      <c r="B9" s="139"/>
-      <c r="C9" s="140"/>
-      <c r="D9" s="140"/>
-      <c r="E9" s="140"/>
-      <c r="F9" s="140"/>
-      <c r="G9" s="141"/>
+      <c r="B9" s="146"/>
+      <c r="C9" s="147"/>
+      <c r="D9" s="147"/>
+      <c r="E9" s="147"/>
+      <c r="F9" s="147"/>
+      <c r="G9" s="148"/>
     </row>
     <row r="10" spans="2:7" ht="55.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="136" t="s">
+      <c r="B10" s="143" t="s">
         <v>115</v>
       </c>
-      <c r="C10" s="137"/>
-      <c r="D10" s="137"/>
-      <c r="E10" s="137"/>
-      <c r="F10" s="137"/>
-      <c r="G10" s="138"/>
+      <c r="C10" s="144"/>
+      <c r="D10" s="144"/>
+      <c r="E10" s="144"/>
+      <c r="F10" s="144"/>
+      <c r="G10" s="145"/>
     </row>
     <row r="11" spans="2:7" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="142"/>
-      <c r="C11" s="143"/>
-      <c r="D11" s="143"/>
-      <c r="E11" s="143"/>
-      <c r="F11" s="143"/>
-      <c r="G11" s="144"/>
+      <c r="B11" s="149"/>
+      <c r="C11" s="150"/>
+      <c r="D11" s="150"/>
+      <c r="E11" s="150"/>
+      <c r="F11" s="150"/>
+      <c r="G11" s="151"/>
     </row>
     <row r="12" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="142"/>
-      <c r="C12" s="143"/>
-      <c r="D12" s="143"/>
-      <c r="E12" s="143"/>
-      <c r="F12" s="143"/>
-      <c r="G12" s="144"/>
+      <c r="B12" s="149"/>
+      <c r="C12" s="150"/>
+      <c r="D12" s="150"/>
+      <c r="E12" s="150"/>
+      <c r="F12" s="150"/>
+      <c r="G12" s="151"/>
     </row>
     <row r="13" spans="2:7" ht="20.25" x14ac:dyDescent="0.2">
-      <c r="B13" s="130"/>
-      <c r="C13" s="131"/>
-      <c r="D13" s="131"/>
-      <c r="E13" s="131"/>
-      <c r="F13" s="131"/>
-      <c r="G13" s="132"/>
+      <c r="B13" s="137"/>
+      <c r="C13" s="138"/>
+      <c r="D13" s="138"/>
+      <c r="E13" s="138"/>
+      <c r="F13" s="138"/>
+      <c r="G13" s="139"/>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B14" s="10"/>
@@ -5801,12 +5840,12 @@
       <c r="G20" s="9"/>
     </row>
     <row r="21" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="B21" s="133"/>
-      <c r="C21" s="134"/>
-      <c r="D21" s="134"/>
-      <c r="E21" s="134"/>
-      <c r="F21" s="134"/>
-      <c r="G21" s="135"/>
+      <c r="B21" s="140"/>
+      <c r="C21" s="141"/>
+      <c r="D21" s="141"/>
+      <c r="E21" s="141"/>
+      <c r="F21" s="141"/>
+      <c r="G21" s="142"/>
       <c r="H21"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
@@ -6108,7 +6147,7 @@
       <c r="D18" s="159"/>
     </row>
     <row r="19" spans="3:4" ht="107.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C19" s="147" t="s">
+      <c r="C19" s="154" t="s">
         <v>44</v>
       </c>
       <c r="D19" s="162"/>
@@ -6236,10 +6275,10 @@
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="66"/>
       <c r="B35" s="67"/>
-      <c r="C35" s="145" t="s">
+      <c r="C35" s="152" t="s">
         <v>73</v>
       </c>
-      <c r="D35" s="146"/>
+      <c r="D35" s="153"/>
     </row>
     <row r="36" spans="1:4" ht="63.75" x14ac:dyDescent="0.2">
       <c r="C36" s="60" t="s">
@@ -6266,75 +6305,81 @@
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C40" s="145" t="s">
+      <c r="C40" s="152" t="s">
         <v>80</v>
       </c>
-      <c r="D40" s="146"/>
+      <c r="D40" s="153"/>
     </row>
     <row r="41" spans="1:4" ht="354.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C41" s="147" t="s">
+      <c r="C41" s="154" t="s">
         <v>81</v>
       </c>
-      <c r="D41" s="148"/>
+      <c r="D41" s="155"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C44" s="145" t="s">
+      <c r="C44" s="152" t="s">
         <v>82</v>
       </c>
-      <c r="D44" s="146"/>
+      <c r="D44" s="153"/>
     </row>
     <row r="45" spans="1:4" ht="360.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C45" s="147" t="s">
+      <c r="C45" s="154" t="s">
         <v>83</v>
       </c>
-      <c r="D45" s="148"/>
+      <c r="D45" s="155"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C46" s="145" t="s">
+      <c r="C46" s="152" t="s">
         <v>84</v>
       </c>
-      <c r="D46" s="146"/>
+      <c r="D46" s="153"/>
     </row>
     <row r="47" spans="1:4" ht="153" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C47" s="147" t="s">
+      <c r="C47" s="154" t="s">
         <v>85</v>
       </c>
-      <c r="D47" s="148"/>
+      <c r="D47" s="155"/>
     </row>
     <row r="50" spans="3:4" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C50" s="155" t="s">
+      <c r="C50" s="169" t="s">
         <v>112</v>
       </c>
-      <c r="D50" s="146"/>
+      <c r="D50" s="153"/>
     </row>
     <row r="51" spans="3:4" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C51" s="149" t="s">
+      <c r="C51" s="163" t="s">
         <v>113</v>
       </c>
-      <c r="D51" s="150"/>
+      <c r="D51" s="164"/>
     </row>
     <row r="52" spans="3:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C52" s="151"/>
-      <c r="D52" s="152"/>
+      <c r="C52" s="165"/>
+      <c r="D52" s="166"/>
     </row>
     <row r="53" spans="3:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C53" s="151"/>
-      <c r="D53" s="152"/>
+      <c r="C53" s="165"/>
+      <c r="D53" s="166"/>
     </row>
     <row r="54" spans="3:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C54" s="151"/>
-      <c r="D54" s="152"/>
+      <c r="C54" s="165"/>
+      <c r="D54" s="166"/>
     </row>
     <row r="55" spans="3:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C55" s="151"/>
-      <c r="D55" s="152"/>
+      <c r="C55" s="165"/>
+      <c r="D55" s="166"/>
     </row>
     <row r="56" spans="3:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C56" s="153"/>
-      <c r="D56" s="154"/>
+      <c r="C56" s="167"/>
+      <c r="D56" s="168"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="C51:D56"/>
+    <mergeCell ref="C50:D50"/>
     <mergeCell ref="C40:D40"/>
     <mergeCell ref="C41:D41"/>
     <mergeCell ref="B1:H1"/>
@@ -6343,12 +6388,6 @@
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="C51:D56"/>
-    <mergeCell ref="C50:D50"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1">
@@ -6372,8 +6411,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:AH177"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7136,10 +7175,10 @@
       <c r="A16" s="106">
         <v>14</v>
       </c>
-      <c r="B16" s="189" t="s">
+      <c r="B16" s="136" t="s">
         <v>266</v>
       </c>
-      <c r="C16" s="183" t="s">
+      <c r="C16" s="130" t="s">
         <v>253</v>
       </c>
       <c r="D16" s="127" t="s">
@@ -7188,7 +7227,7 @@
       <c r="A17" s="106">
         <v>15</v>
       </c>
-      <c r="B17" s="189" t="s">
+      <c r="B17" s="136" t="s">
         <v>267</v>
       </c>
       <c r="C17" s="127" t="s">
@@ -7240,7 +7279,7 @@
       <c r="A18" s="106">
         <v>16</v>
       </c>
-      <c r="B18" s="189" t="s">
+      <c r="B18" s="136" t="s">
         <v>268</v>
       </c>
       <c r="C18" s="127" t="s">
@@ -7292,10 +7331,10 @@
       <c r="A19" s="106">
         <v>17</v>
       </c>
-      <c r="B19" s="189" t="s">
+      <c r="B19" s="136" t="s">
         <v>269</v>
       </c>
-      <c r="C19" s="184" t="s">
+      <c r="C19" s="131" t="s">
         <v>254</v>
       </c>
       <c r="D19" s="127" t="s">
@@ -7344,10 +7383,10 @@
       <c r="A20" s="106">
         <v>18</v>
       </c>
-      <c r="B20" s="189" t="s">
+      <c r="B20" s="136" t="s">
         <v>270</v>
       </c>
-      <c r="C20" s="184" t="s">
+      <c r="C20" s="131" t="s">
         <v>255</v>
       </c>
       <c r="D20" s="127" t="s">
@@ -7396,10 +7435,10 @@
       <c r="A21" s="106">
         <v>19</v>
       </c>
-      <c r="B21" s="189" t="s">
+      <c r="B21" s="136" t="s">
         <v>271</v>
       </c>
-      <c r="C21" s="184" t="s">
+      <c r="C21" s="131" t="s">
         <v>256</v>
       </c>
       <c r="D21" s="127" t="s">
@@ -7448,10 +7487,10 @@
       <c r="A22" s="106">
         <v>20</v>
       </c>
-      <c r="B22" s="189" t="s">
+      <c r="B22" s="136" t="s">
         <v>272</v>
       </c>
-      <c r="C22" s="184" t="s">
+      <c r="C22" s="131" t="s">
         <v>257</v>
       </c>
       <c r="D22" s="127" t="s">
@@ -7500,10 +7539,10 @@
       <c r="A23" s="106">
         <v>21</v>
       </c>
-      <c r="B23" s="189" t="s">
+      <c r="B23" s="136" t="s">
         <v>273</v>
       </c>
-      <c r="C23" s="184" t="s">
+      <c r="C23" s="131" t="s">
         <v>258</v>
       </c>
       <c r="D23" s="127" t="s">
@@ -7552,10 +7591,10 @@
       <c r="A24" s="106">
         <v>22</v>
       </c>
-      <c r="B24" s="189" t="s">
+      <c r="B24" s="136" t="s">
         <v>274</v>
       </c>
-      <c r="C24" s="184" t="s">
+      <c r="C24" s="131" t="s">
         <v>259</v>
       </c>
       <c r="D24" s="127" t="s">
@@ -7604,10 +7643,10 @@
       <c r="A25" s="106">
         <v>23</v>
       </c>
-      <c r="B25" s="189" t="s">
+      <c r="B25" s="136" t="s">
         <v>275</v>
       </c>
-      <c r="C25" s="184" t="s">
+      <c r="C25" s="131" t="s">
         <v>260</v>
       </c>
       <c r="D25" s="127" t="s">
@@ -7656,10 +7695,10 @@
       <c r="A26" s="106">
         <v>24</v>
       </c>
-      <c r="B26" s="189" t="s">
+      <c r="B26" s="136" t="s">
         <v>276</v>
       </c>
-      <c r="C26" s="184" t="s">
+      <c r="C26" s="131" t="s">
         <v>261</v>
       </c>
       <c r="D26" s="127" t="s">
@@ -7708,10 +7747,10 @@
       <c r="A27" s="106">
         <v>25</v>
       </c>
-      <c r="B27" s="189" t="s">
+      <c r="B27" s="136" t="s">
         <v>277</v>
       </c>
-      <c r="C27" s="184" t="s">
+      <c r="C27" s="131" t="s">
         <v>262</v>
       </c>
       <c r="D27" s="127" t="s">
@@ -7760,10 +7799,10 @@
       <c r="A28" s="106">
         <v>26</v>
       </c>
-      <c r="B28" s="189" t="s">
+      <c r="B28" s="136" t="s">
         <v>278</v>
       </c>
-      <c r="C28" s="184" t="s">
+      <c r="C28" s="131" t="s">
         <v>263</v>
       </c>
       <c r="D28" s="127" t="s">
@@ -9390,7 +9429,9 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:AP186"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="N30" sqref="N30"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -9472,11 +9513,11 @@
       <c r="O2" s="103" t="s">
         <v>71</v>
       </c>
-      <c r="P2" s="163" t="s">
+      <c r="P2" s="170" t="s">
         <v>73</v>
       </c>
-      <c r="Q2" s="163"/>
-      <c r="R2" s="163"/>
+      <c r="Q2" s="170"/>
+      <c r="R2" s="170"/>
       <c r="S2" s="104"/>
       <c r="T2" s="104"/>
       <c r="U2" s="104"/>
@@ -9582,15 +9623,19 @@
         <v>127</v>
       </c>
       <c r="K4" s="108" t="s">
-        <v>89</v>
+        <v>279</v>
       </c>
       <c r="L4" s="108" t="s">
         <v>90</v>
       </c>
-      <c r="M4" s="108"/>
-      <c r="N4" s="108"/>
+      <c r="M4" s="190">
+        <v>0.2</v>
+      </c>
+      <c r="N4" s="190">
+        <v>0.2</v>
+      </c>
       <c r="O4" s="108" t="s">
-        <v>124</v>
+        <v>279</v>
       </c>
       <c r="P4" s="110">
         <f t="shared" ref="P4:P16" si="0">IF(K4="X",IF(O4="Complete",N4,0),0)</f>
@@ -9602,7 +9647,7 @@
       </c>
       <c r="R4" s="111">
         <f t="shared" ref="R4:R16" si="2">IF(K4&lt;&gt;"X",IF(O4="Complete",N4,0),0)</f>
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="S4" s="104"/>
       <c r="T4" s="104"/>
@@ -9660,15 +9705,19 @@
         <v>170</v>
       </c>
       <c r="K5" s="108" t="s">
-        <v>89</v>
+        <v>279</v>
       </c>
       <c r="L5" s="108" t="s">
         <v>90</v>
       </c>
-      <c r="M5" s="108"/>
-      <c r="N5" s="108"/>
+      <c r="M5" s="190">
+        <v>0.3</v>
+      </c>
+      <c r="N5" s="190">
+        <v>0.3</v>
+      </c>
       <c r="O5" s="108" t="s">
-        <v>124</v>
+        <v>279</v>
       </c>
       <c r="P5" s="110">
         <f t="shared" si="0"/>
@@ -9680,7 +9729,7 @@
       </c>
       <c r="R5" s="111">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="S5" s="104"/>
       <c r="T5" s="104"/>
@@ -9738,15 +9787,19 @@
         <v>130</v>
       </c>
       <c r="K6" s="108" t="s">
-        <v>89</v>
+        <v>279</v>
       </c>
       <c r="L6" s="108" t="s">
         <v>90</v>
       </c>
-      <c r="M6" s="108"/>
-      <c r="N6" s="108"/>
+      <c r="M6" s="190">
+        <v>0.2</v>
+      </c>
+      <c r="N6" s="190">
+        <v>0.2</v>
+      </c>
       <c r="O6" s="108" t="s">
-        <v>124</v>
+        <v>279</v>
       </c>
       <c r="P6" s="110">
         <f t="shared" si="0"/>
@@ -9758,7 +9811,7 @@
       </c>
       <c r="R6" s="111">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="S6" s="69"/>
       <c r="T6" s="69"/>
@@ -9816,15 +9869,19 @@
         <v>193</v>
       </c>
       <c r="K7" s="108" t="s">
-        <v>89</v>
+        <v>279</v>
       </c>
       <c r="L7" s="109" t="s">
         <v>90</v>
       </c>
-      <c r="M7" s="108"/>
-      <c r="N7" s="108"/>
+      <c r="M7" s="190">
+        <v>0.1</v>
+      </c>
+      <c r="N7" s="190">
+        <v>0.1</v>
+      </c>
       <c r="O7" s="108" t="s">
-        <v>124</v>
+        <v>279</v>
       </c>
       <c r="P7" s="110">
         <f t="shared" si="0"/>
@@ -9836,7 +9893,7 @@
       </c>
       <c r="R7" s="111">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="S7" s="69"/>
       <c r="T7" s="69"/>
@@ -9894,15 +9951,19 @@
         <v>132</v>
       </c>
       <c r="K8" s="108" t="s">
-        <v>89</v>
+        <v>279</v>
       </c>
       <c r="L8" s="108" t="s">
         <v>90</v>
       </c>
-      <c r="M8" s="108"/>
-      <c r="N8" s="108"/>
+      <c r="M8" s="190">
+        <v>0.2</v>
+      </c>
+      <c r="N8" s="190">
+        <v>0.2</v>
+      </c>
       <c r="O8" s="108" t="s">
-        <v>124</v>
+        <v>279</v>
       </c>
       <c r="P8" s="110">
         <v>0</v>
@@ -9969,15 +10030,19 @@
         <v>171</v>
       </c>
       <c r="K9" s="108" t="s">
-        <v>89</v>
+        <v>279</v>
       </c>
       <c r="L9" s="108" t="s">
         <v>90</v>
       </c>
-      <c r="M9" s="108"/>
-      <c r="N9" s="108"/>
+      <c r="M9" s="190">
+        <v>0.2</v>
+      </c>
+      <c r="N9" s="190">
+        <v>0.2</v>
+      </c>
       <c r="O9" s="108" t="s">
-        <v>124</v>
+        <v>279</v>
       </c>
       <c r="P9" s="110">
         <f t="shared" si="0"/>
@@ -9989,7 +10054,7 @@
       </c>
       <c r="R9" s="111">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="S9" s="69"/>
       <c r="T9" s="69"/>
@@ -10047,15 +10112,19 @@
         <v>173</v>
       </c>
       <c r="K10" s="108" t="s">
-        <v>89</v>
+        <v>279</v>
       </c>
       <c r="L10" s="108" t="s">
         <v>90</v>
       </c>
-      <c r="M10" s="108"/>
-      <c r="N10" s="108"/>
+      <c r="M10" s="190">
+        <v>0.3</v>
+      </c>
+      <c r="N10" s="190">
+        <v>0.3</v>
+      </c>
       <c r="O10" s="108" t="s">
-        <v>124</v>
+        <v>279</v>
       </c>
       <c r="P10" s="110">
         <f t="shared" si="0"/>
@@ -10067,7 +10136,7 @@
       </c>
       <c r="R10" s="111">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="S10" s="69"/>
       <c r="T10" s="69"/>
@@ -10125,15 +10194,19 @@
         <v>176</v>
       </c>
       <c r="K11" s="108" t="s">
-        <v>89</v>
+        <v>279</v>
       </c>
       <c r="L11" s="109" t="s">
         <v>92</v>
       </c>
-      <c r="M11" s="108"/>
-      <c r="N11" s="108"/>
+      <c r="M11" s="190">
+        <v>0.4</v>
+      </c>
+      <c r="N11" s="190">
+        <v>0.4</v>
+      </c>
       <c r="O11" s="108" t="s">
-        <v>124</v>
+        <v>279</v>
       </c>
       <c r="P11" s="110">
         <f t="shared" si="0"/>
@@ -10145,7 +10218,7 @@
       </c>
       <c r="R11" s="111">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="S11" s="69"/>
       <c r="T11" s="69"/>
@@ -10203,15 +10276,19 @@
         <v>180</v>
       </c>
       <c r="K12" s="108" t="s">
-        <v>89</v>
+        <v>279</v>
       </c>
       <c r="L12" s="109" t="s">
         <v>92</v>
       </c>
-      <c r="M12" s="108"/>
-      <c r="N12" s="108"/>
+      <c r="M12" s="190">
+        <v>0.2</v>
+      </c>
+      <c r="N12" s="190">
+        <v>0.2</v>
+      </c>
       <c r="O12" s="108" t="s">
-        <v>124</v>
+        <v>279</v>
       </c>
       <c r="P12" s="110">
         <f t="shared" si="0"/>
@@ -10223,7 +10300,7 @@
       </c>
       <c r="R12" s="111">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="S12" s="69"/>
       <c r="T12" s="69"/>
@@ -10281,13 +10358,17 @@
         <v>181</v>
       </c>
       <c r="K13" s="108" t="s">
-        <v>89</v>
+        <v>279</v>
       </c>
       <c r="L13" s="109" t="s">
         <v>92</v>
       </c>
-      <c r="M13" s="108"/>
-      <c r="N13" s="108"/>
+      <c r="M13" s="190">
+        <v>0.1</v>
+      </c>
+      <c r="N13" s="190">
+        <v>0.1</v>
+      </c>
       <c r="O13" s="108" t="s">
         <v>124</v>
       </c>
@@ -10297,7 +10378,7 @@
       </c>
       <c r="Q13" s="111">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="R13" s="111">
         <f t="shared" si="2"/>
@@ -10359,15 +10440,19 @@
         <v>192</v>
       </c>
       <c r="K14" s="108" t="s">
-        <v>89</v>
+        <v>279</v>
       </c>
       <c r="L14" s="109" t="s">
         <v>92</v>
       </c>
-      <c r="M14" s="108"/>
-      <c r="N14" s="108"/>
+      <c r="M14" s="190">
+        <v>0.2</v>
+      </c>
+      <c r="N14" s="190">
+        <v>0.2</v>
+      </c>
       <c r="O14" s="108" t="s">
-        <v>124</v>
+        <v>279</v>
       </c>
       <c r="P14" s="110">
         <f t="shared" si="0"/>
@@ -10379,7 +10464,7 @@
       </c>
       <c r="R14" s="111">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="S14" s="69"/>
       <c r="T14" s="69"/>
@@ -10437,15 +10522,19 @@
         <v>186</v>
       </c>
       <c r="K15" s="108" t="s">
-        <v>89</v>
+        <v>279</v>
       </c>
       <c r="L15" s="109" t="s">
         <v>92</v>
       </c>
-      <c r="M15" s="108"/>
-      <c r="N15" s="108"/>
+      <c r="M15" s="190">
+        <v>0.5</v>
+      </c>
+      <c r="N15" s="190">
+        <v>0.5</v>
+      </c>
       <c r="O15" s="108" t="s">
-        <v>124</v>
+        <v>279</v>
       </c>
       <c r="P15" s="110">
         <f t="shared" si="0"/>
@@ -10457,7 +10546,7 @@
       </c>
       <c r="R15" s="111">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="S15" s="69"/>
       <c r="T15" s="69"/>
@@ -10511,19 +10600,23 @@
       <c r="I16" s="129" t="s">
         <v>197</v>
       </c>
-      <c r="J16" s="186" t="s">
+      <c r="J16" s="133" t="s">
         <v>190</v>
       </c>
       <c r="K16" s="108" t="s">
-        <v>89</v>
+        <v>279</v>
       </c>
       <c r="L16" s="109" t="s">
         <v>92</v>
       </c>
-      <c r="M16" s="108"/>
-      <c r="N16" s="108"/>
+      <c r="M16" s="190">
+        <v>0.2</v>
+      </c>
+      <c r="N16" s="190">
+        <v>0.2</v>
+      </c>
       <c r="O16" s="108" t="s">
-        <v>124</v>
+        <v>279</v>
       </c>
       <c r="P16" s="110">
         <f t="shared" si="0"/>
@@ -10535,7 +10628,7 @@
       </c>
       <c r="R16" s="111">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="S16" s="69"/>
       <c r="T16" s="69"/>
@@ -10586,22 +10679,26 @@
       <c r="H17" s="109" t="s">
         <v>225</v>
       </c>
-      <c r="I17" s="187" t="s">
+      <c r="I17" s="134" t="s">
         <v>199</v>
       </c>
       <c r="J17" s="127" t="s">
         <v>238</v>
       </c>
       <c r="K17" s="108" t="s">
-        <v>89</v>
+        <v>279</v>
       </c>
       <c r="L17" s="109" t="s">
         <v>92</v>
       </c>
-      <c r="M17" s="108"/>
-      <c r="N17" s="108"/>
+      <c r="M17" s="190">
+        <v>0.2</v>
+      </c>
+      <c r="N17" s="190">
+        <v>0.2</v>
+      </c>
       <c r="O17" s="108" t="s">
-        <v>124</v>
+        <v>279</v>
       </c>
       <c r="P17" s="110">
         <f t="shared" ref="P17:P28" si="3">IF(K17="X",IF(O17="Complete",N17,0),0)</f>
@@ -10613,7 +10710,7 @@
       </c>
       <c r="R17" s="111">
         <f t="shared" ref="R17:R28" si="5">IF(K17&lt;&gt;"X",IF(O17="Complete",N17,0),0)</f>
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="S17" s="69"/>
       <c r="T17" s="69"/>
@@ -10664,22 +10761,26 @@
       <c r="H18" s="109" t="s">
         <v>226</v>
       </c>
-      <c r="I18" s="188" t="s">
+      <c r="I18" s="135" t="s">
         <v>200</v>
       </c>
       <c r="J18" s="127" t="s">
         <v>239</v>
       </c>
       <c r="K18" s="108" t="s">
-        <v>89</v>
+        <v>279</v>
       </c>
       <c r="L18" s="109" t="s">
         <v>92</v>
       </c>
-      <c r="M18" s="108"/>
-      <c r="N18" s="108"/>
+      <c r="M18" s="190">
+        <v>0.3</v>
+      </c>
+      <c r="N18" s="190">
+        <v>0.3</v>
+      </c>
       <c r="O18" s="108" t="s">
-        <v>124</v>
+        <v>279</v>
       </c>
       <c r="P18" s="110">
         <f t="shared" si="3"/>
@@ -10691,7 +10792,7 @@
       </c>
       <c r="R18" s="111">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="S18" s="69"/>
       <c r="T18" s="69"/>
@@ -10742,22 +10843,26 @@
       <c r="H19" s="109" t="s">
         <v>227</v>
       </c>
-      <c r="I19" s="185" t="s">
+      <c r="I19" s="132" t="s">
         <v>201</v>
       </c>
       <c r="J19" s="127" t="s">
         <v>240</v>
       </c>
       <c r="K19" s="108" t="s">
-        <v>89</v>
+        <v>279</v>
       </c>
       <c r="L19" s="109" t="s">
         <v>92</v>
       </c>
-      <c r="M19" s="108"/>
-      <c r="N19" s="108"/>
+      <c r="M19" s="190">
+        <v>0.3</v>
+      </c>
+      <c r="N19" s="190">
+        <v>0.3</v>
+      </c>
       <c r="O19" s="108" t="s">
-        <v>124</v>
+        <v>279</v>
       </c>
       <c r="P19" s="110">
         <f t="shared" si="3"/>
@@ -10769,7 +10874,7 @@
       </c>
       <c r="R19" s="111">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="S19" s="69"/>
       <c r="T19" s="69"/>
@@ -10820,22 +10925,26 @@
       <c r="H20" s="109" t="s">
         <v>228</v>
       </c>
-      <c r="I20" s="185" t="s">
+      <c r="I20" s="132" t="s">
         <v>202</v>
       </c>
       <c r="J20" s="127" t="s">
         <v>241</v>
       </c>
       <c r="K20" s="108" t="s">
-        <v>89</v>
+        <v>279</v>
       </c>
       <c r="L20" s="109" t="s">
         <v>92</v>
       </c>
-      <c r="M20" s="108"/>
-      <c r="N20" s="108"/>
+      <c r="M20" s="190">
+        <v>0.2</v>
+      </c>
+      <c r="N20" s="190">
+        <v>0.2</v>
+      </c>
       <c r="O20" s="108" t="s">
-        <v>124</v>
+        <v>279</v>
       </c>
       <c r="P20" s="110">
         <f t="shared" si="3"/>
@@ -10847,7 +10956,7 @@
       </c>
       <c r="R20" s="111">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="S20" s="69"/>
       <c r="T20" s="69"/>
@@ -10898,19 +11007,21 @@
       <c r="H21" s="109" t="s">
         <v>229</v>
       </c>
-      <c r="I21" s="185" t="s">
+      <c r="I21" s="132" t="s">
         <v>203</v>
       </c>
       <c r="J21" s="127" t="s">
         <v>242</v>
       </c>
       <c r="K21" s="108" t="s">
-        <v>89</v>
+        <v>124</v>
       </c>
       <c r="L21" s="109" t="s">
         <v>92</v>
       </c>
-      <c r="M21" s="108"/>
+      <c r="M21" s="92">
+        <v>0</v>
+      </c>
       <c r="N21" s="108"/>
       <c r="O21" s="108" t="s">
         <v>124</v>
@@ -10976,14 +11087,14 @@
       <c r="H22" s="109" t="s">
         <v>230</v>
       </c>
-      <c r="I22" s="185" t="s">
+      <c r="I22" s="132" t="s">
         <v>204</v>
       </c>
       <c r="J22" s="127" t="s">
         <v>243</v>
       </c>
       <c r="K22" s="108" t="s">
-        <v>89</v>
+        <v>124</v>
       </c>
       <c r="L22" s="109" t="s">
         <v>92</v>
@@ -11054,7 +11165,7 @@
       <c r="H23" s="109" t="s">
         <v>231</v>
       </c>
-      <c r="I23" s="185" t="s">
+      <c r="I23" s="132" t="s">
         <v>205</v>
       </c>
       <c r="J23" s="127" t="s">
@@ -11132,7 +11243,7 @@
       <c r="H24" s="109" t="s">
         <v>232</v>
       </c>
-      <c r="I24" s="185" t="s">
+      <c r="I24" s="132" t="s">
         <v>206</v>
       </c>
       <c r="J24" s="127" t="s">
@@ -11210,7 +11321,7 @@
       <c r="H25" s="109" t="s">
         <v>233</v>
       </c>
-      <c r="I25" s="185" t="s">
+      <c r="I25" s="132" t="s">
         <v>207</v>
       </c>
       <c r="J25" s="127" t="s">
@@ -11288,7 +11399,7 @@
       <c r="H26" s="109" t="s">
         <v>234</v>
       </c>
-      <c r="I26" s="185" t="s">
+      <c r="I26" s="132" t="s">
         <v>208</v>
       </c>
       <c r="J26" s="127" t="s">
@@ -11366,7 +11477,7 @@
       <c r="H27" s="109" t="s">
         <v>235</v>
       </c>
-      <c r="I27" s="185" t="s">
+      <c r="I27" s="132" t="s">
         <v>209</v>
       </c>
       <c r="J27" s="127" t="s">
@@ -11444,22 +11555,26 @@
       <c r="H28" s="109" t="s">
         <v>236</v>
       </c>
-      <c r="I28" s="185" t="s">
+      <c r="I28" s="132" t="s">
         <v>210</v>
       </c>
       <c r="J28" s="127" t="s">
         <v>249</v>
       </c>
       <c r="K28" s="108" t="s">
-        <v>89</v>
+        <v>279</v>
       </c>
       <c r="L28" s="109" t="s">
         <v>92</v>
       </c>
-      <c r="M28" s="108"/>
-      <c r="N28" s="108"/>
+      <c r="M28" s="190">
+        <v>0.1</v>
+      </c>
+      <c r="N28" s="108">
+        <v>0.1</v>
+      </c>
       <c r="O28" s="108" t="s">
-        <v>124</v>
+        <v>279</v>
       </c>
       <c r="P28" s="110">
         <f t="shared" si="3"/>
@@ -11471,7 +11586,7 @@
       </c>
       <c r="R28" s="111">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="S28" s="69"/>
       <c r="T28" s="69"/>
@@ -11522,7 +11637,7 @@
       <c r="H29" s="109" t="s">
         <v>237</v>
       </c>
-      <c r="I29" s="185" t="s">
+      <c r="I29" s="132" t="s">
         <v>211</v>
       </c>
       <c r="J29" s="127" t="s">
@@ -11592,8 +11707,8 @@
       </c>
       <c r="M30" s="86"/>
       <c r="N30" s="87">
-        <f>SUM(N4:N16)</f>
-        <v>0</v>
+        <f>SUM(N4:N20)</f>
+        <v>4.1000000000000005</v>
       </c>
       <c r="O30" s="85"/>
       <c r="AP30" s="83"/>
@@ -14268,7 +14383,7 @@
     <mergeCell ref="B1:I1"/>
   </mergeCells>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O4:O29">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O4:O29 K4:K22 K28">
       <formula1>"Proposed, Assigned, Inprogress, Complete, Cancelled"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L40:M65542 N117:N65542 C30:C65542 F30:F65542 D31:E65542">
@@ -14324,7 +14439,7 @@
   <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="A5" sqref="A5:G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -14352,15 +14467,15 @@
       <c r="O1" s="56"/>
     </row>
     <row r="2" spans="1:15" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="164" t="s">
+      <c r="A2" s="171" t="s">
         <v>96</v>
       </c>
-      <c r="B2" s="165"/>
-      <c r="C2" s="165"/>
-      <c r="D2" s="165"/>
-      <c r="E2" s="165"/>
-      <c r="F2" s="166"/>
-      <c r="G2" s="166"/>
+      <c r="B2" s="172"/>
+      <c r="C2" s="172"/>
+      <c r="D2" s="172"/>
+      <c r="E2" s="172"/>
+      <c r="F2" s="173"/>
+      <c r="G2" s="173"/>
     </row>
     <row r="3" spans="1:15" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A3" s="93" t="s">
@@ -14396,7 +14511,7 @@
       </c>
       <c r="D4" s="95">
         <f>'Product - Release Tracking'!N30-E4-G4</f>
-        <v>0</v>
+        <v>3.9000000000000004</v>
       </c>
       <c r="E4" s="95">
         <f>SUMIF('Product - Release Tracking'!A$4:A$16,'Report Data'!B4,'Product - Release Tracking'!P$4:P$16)</f>
@@ -14407,7 +14522,7 @@
       </c>
       <c r="G4" s="95">
         <f>SUMIF('Product - Release Tracking'!A$4:A$16,'Report Data'!B4,'Product - Release Tracking'!R$4:R$16)</f>
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
@@ -14423,7 +14538,7 @@
       </c>
       <c r="D5" s="95">
         <f>D4-E5-G5</f>
-        <v>0</v>
+        <v>3.6000000000000005</v>
       </c>
       <c r="E5" s="95">
         <f>SUMIF('Product - Release Tracking'!A$4:A$16,'Report Data'!B5,'Product - Release Tracking'!P$4:P$16)</f>
@@ -14434,7 +14549,7 @@
       </c>
       <c r="G5" s="95">
         <f>SUMIF('Product - Release Tracking'!A$4:A$16,'Report Data'!B5,'Product - Release Tracking'!R$4:R$16)</f>
-        <v>0</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
@@ -14451,7 +14566,7 @@
       </c>
       <c r="D6" s="95">
         <f>D5-E6-G6</f>
-        <v>0</v>
+        <v>3.6000000000000005</v>
       </c>
       <c r="E6" s="95">
         <f>SUMIF('Product - Release Tracking'!A$4:A$16,'Report Data'!B6,'Product - Release Tracking'!P$4:P$16)</f>
@@ -14481,7 +14596,7 @@
       </c>
       <c r="D7" s="95">
         <f>D6-E7-G7</f>
-        <v>0</v>
+        <v>3.6000000000000005</v>
       </c>
       <c r="E7" s="95">
         <f>SUMIF('Product - Release Tracking'!A$4:A$16,'Report Data'!B7,'Product - Release Tracking'!P$4:P$16)</f>
@@ -14567,27 +14682,27 @@
   <sheetData>
     <row r="1" spans="1:10" s="97" customFormat="1" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="96"/>
-      <c r="B1" s="167" t="s">
+      <c r="B1" s="174" t="s">
         <v>169</v>
       </c>
-      <c r="C1" s="168"/>
-      <c r="D1" s="168"/>
-      <c r="E1" s="168"/>
-      <c r="F1" s="169"/>
+      <c r="C1" s="175"/>
+      <c r="D1" s="175"/>
+      <c r="E1" s="175"/>
+      <c r="F1" s="176"/>
     </row>
     <row r="2" spans="1:10" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="4" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="B4" s="98"/>
-      <c r="C4" s="170" t="s">
+      <c r="C4" s="177" t="s">
         <v>103</v>
       </c>
-      <c r="D4" s="170"/>
-      <c r="E4" s="170"/>
-      <c r="F4" s="170"/>
-      <c r="G4" s="171"/>
-      <c r="H4" s="171"/>
-      <c r="I4" s="171"/>
-      <c r="J4" s="171"/>
+      <c r="D4" s="177"/>
+      <c r="E4" s="177"/>
+      <c r="F4" s="177"/>
+      <c r="G4" s="178"/>
+      <c r="H4" s="178"/>
+      <c r="I4" s="178"/>
+      <c r="J4" s="178"/>
     </row>
     <row r="5" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B5" s="37" t="s">
@@ -14875,14 +14990,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="49" customFormat="1" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="172" t="s">
+      <c r="A1" s="179" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="172"/>
-      <c r="C1" s="172"/>
-      <c r="D1" s="172"/>
-      <c r="E1" s="172"/>
-      <c r="F1" s="173"/>
+      <c r="B1" s="179"/>
+      <c r="C1" s="179"/>
+      <c r="D1" s="179"/>
+      <c r="E1" s="179"/>
+      <c r="F1" s="180"/>
     </row>
     <row r="2" spans="1:6" s="33" customFormat="1" ht="24" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="31"/>
@@ -14892,13 +15007,13 @@
       <c r="E2" s="32"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="174" t="s">
+      <c r="A3" s="181" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="174"/>
-      <c r="C3" s="174"/>
-      <c r="D3" s="174"/>
-      <c r="E3" s="174"/>
+      <c r="B3" s="181"/>
+      <c r="C3" s="181"/>
+      <c r="D3" s="181"/>
+      <c r="E3" s="181"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="34"/>
@@ -14907,26 +15022,26 @@
       <c r="A5" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="177" t="s">
+      <c r="B5" s="184" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="178"/>
-      <c r="D5" s="178"/>
-      <c r="E5" s="179"/>
+      <c r="C5" s="185"/>
+      <c r="D5" s="185"/>
+      <c r="E5" s="186"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="180" t="s">
+      <c r="B6" s="187" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="181"/>
-      <c r="D6" s="181"/>
-      <c r="E6" s="182"/>
+      <c r="C6" s="188"/>
+      <c r="D6" s="188"/>
+      <c r="E6" s="189"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="175" t="s">
+      <c r="A7" s="182" t="s">
         <v>16</v>
       </c>
       <c r="B7" s="45" t="s">
@@ -14943,35 +15058,35 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="175"/>
+      <c r="A8" s="182"/>
       <c r="B8" s="36"/>
       <c r="C8" s="36"/>
       <c r="D8" s="48"/>
       <c r="E8" s="36"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="175"/>
+      <c r="A9" s="182"/>
       <c r="B9" s="36"/>
       <c r="C9" s="36"/>
       <c r="D9" s="48"/>
       <c r="E9" s="36"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="175"/>
+      <c r="A10" s="182"/>
       <c r="B10" s="36"/>
       <c r="C10" s="36"/>
       <c r="D10" s="48"/>
       <c r="E10" s="36"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="176"/>
+      <c r="A11" s="183"/>
       <c r="B11" s="36"/>
       <c r="C11" s="36"/>
       <c r="D11" s="48"/>
       <c r="E11" s="36"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="175" t="s">
+      <c r="A12" s="182" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="45" t="s">
@@ -14988,28 +15103,28 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="175"/>
+      <c r="A13" s="182"/>
       <c r="B13" s="36"/>
       <c r="C13" s="36"/>
       <c r="D13" s="48"/>
       <c r="E13" s="36"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="175"/>
+      <c r="A14" s="182"/>
       <c r="B14" s="36"/>
       <c r="C14" s="36"/>
       <c r="D14" s="48"/>
       <c r="E14" s="36"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="175"/>
+      <c r="A15" s="182"/>
       <c r="B15" s="36"/>
       <c r="C15" s="36"/>
       <c r="D15" s="48"/>
       <c r="E15" s="36"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="176"/>
+      <c r="A16" s="183"/>
       <c r="B16" s="36"/>
       <c r="C16" s="36"/>
       <c r="D16" s="48"/>
@@ -15034,9 +15149,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties">
-  <LongProp xmlns="" name="PIPDescription"><![CDATA[Agile Process has been updated with Daikibo and SAFe framework. Accordingly the following artifacts are updated with Agile Release Plan Generator Product Backlog Checklist for Release Planning Agile Metrics Model Tailoring Guideline - Cognizant Agile Process Guideline for Daikibo Framework]]></LongProp>
-</LongProperties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -15211,12 +15329,9 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties">
+  <LongProp xmlns="" name="PIPDescription"><![CDATA[Agile Process has been updated with Daikibo and SAFe framework. Accordingly the following artifacts are updated with Agile Release Plan Generator Product Backlog Checklist for Release Planning Agile Metrics Model Tailoring Guideline - Cognizant Agile Process Guideline for Daikibo Framework]]></LongProp>
+</LongProperties>
 </file>
 
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
@@ -15234,22 +15349,37 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3480BB77-980B-43DC-A421-1032363DCF0E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13F11D9D-C7B8-4288-8F9C-B4F01751BE56}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
-    <ds:schemaRef ds:uri=""/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F7464A78-F4D3-46E5-8BE9-35BF4A1F14AD}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F7464A78-F4D3-46E5-8BE9-35BF4A1F14AD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="eac52b12-2228-488c-9d59-8a93d308b64e"/>
+    <ds:schemaRef ds:uri="951c5514-b77c-4532-82d5-a05f2f7d58e2"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13F11D9D-C7B8-4288-8F9C-B4F01751BE56}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3480BB77-980B-43DC-A421-1032363DCF0E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+    <ds:schemaRef ds:uri=""/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -15266,6 +15396,7 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="5349db9c-67ed-4999-a121-efc56dbedff2"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="951c5514-b77c-4532-82d5-a05f2f7d58e2"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>